<commit_message>
Updating Weight Measurement schema and documentation
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>WeightID</t>
   </si>
@@ -38,10 +38,13 @@
     <t>Weight (Kg)</t>
   </si>
   <si>
-    <t>Weight Pounds</t>
-  </si>
-  <si>
-    <t>Gain/Loss Amount</t>
+    <t>TotalToTarget (lbs)</t>
+  </si>
+  <si>
+    <t>Weight (lbs)</t>
+  </si>
+  <si>
+    <t>Gain/Loss Amount (lbs)</t>
   </si>
 </sst>
 </file>
@@ -49,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,7 +86,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -412,10 +415,11 @@
     <col min="3" max="3" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -429,13 +433,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -454,13 +461,17 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
+      <c r="G2" s="2">
+        <f>E2-210</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>43095</v>
+        <v>43101</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -468,46 +479,6 @@
       <c r="F3" s="2">
         <f>E3-E2</f>
         <v>-231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43096</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43097</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43098</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Id to sleep and removing redundant weight measurement
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,21 +466,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43101</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <f>E3-E2</f>
-        <v>-231</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding updated WeightMeasurements 8/02/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>WeightID</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>15.11</t>
+  </si>
+  <si>
+    <t>15.08</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>E2-210</f>
+        <f t="shared" ref="G2:G8" si="0">E2-210</f>
         <v>21</v>
       </c>
     </row>
@@ -491,7 +494,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="2">
-        <f>E3-210</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -516,7 +519,7 @@
         <v>-4.0999999999999943</v>
       </c>
       <c r="G4" s="2">
-        <f>E4-210</f>
+        <f t="shared" si="0"/>
         <v>15.900000000000006</v>
       </c>
     </row>
@@ -541,7 +544,7 @@
         <v>-3.0999999999999943</v>
       </c>
       <c r="G5" s="2">
-        <f>E5-210</f>
+        <f t="shared" si="0"/>
         <v>12.800000000000011</v>
       </c>
     </row>
@@ -566,7 +569,7 @@
         <v>-1.9000000000000057</v>
       </c>
       <c r="G6" s="2">
-        <f>E6-210</f>
+        <f t="shared" si="0"/>
         <v>10.900000000000006</v>
       </c>
     </row>
@@ -591,8 +594,33 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <f>E7-210</f>
+        <f t="shared" si="0"/>
         <v>10.900000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43139</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>99</v>
+      </c>
+      <c r="E8" s="2">
+        <v>218</v>
+      </c>
+      <c r="F8" s="2">
+        <f>E8-E7</f>
+        <v>-2.9000000000000057</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding BMI formula to dataset
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7194D02-2C4D-41BB-9F09-F48B810AD086}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FE5A61-5AE5-4725-A79A-280E5A1B12C8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -471,7 +471,8 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
+        <f>ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
     </row>
@@ -495,8 +496,9 @@
         <f t="shared" ref="F3:F13" si="0">E3-E2</f>
         <v>-1</v>
       </c>
-      <c r="G3" s="2">
-        <v>29.43</v>
+      <c r="G3">
+        <f>ROUND((D3/1.88)/1.88,2)</f>
+        <v>29.62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -519,8 +521,9 @@
         <f t="shared" si="0"/>
         <v>-4.0999999999999943</v>
       </c>
-      <c r="G4" s="2">
-        <v>28.86</v>
+      <c r="G4">
+        <f>ROUND((D4/1.88)/1.88,2)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -543,8 +546,9 @@
         <f t="shared" si="0"/>
         <v>-3.0999999999999943</v>
       </c>
-      <c r="G5" s="2">
-        <v>28.58</v>
+      <c r="G5">
+        <f>ROUND((D5/1.88)/1.88,2)</f>
+        <v>28.6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -567,8 +571,9 @@
         <f t="shared" si="0"/>
         <v>-1.9000000000000057</v>
       </c>
-      <c r="G6" s="2">
-        <v>28.29</v>
+      <c r="G6">
+        <f>ROUND((D6/1.88)/1.88,2)</f>
+        <v>28.35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -591,8 +596,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="2">
-        <v>28.29</v>
+      <c r="G7">
+        <f>ROUND((D7/1.88)/1.88,2)</f>
+        <v>28.35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -615,7 +621,8 @@
         <f t="shared" si="0"/>
         <v>-2.9000000000000057</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
+        <f>ROUND((D8/1.88)/1.88,2)</f>
         <v>28.01</v>
       </c>
     </row>
@@ -639,8 +646,9 @@
         <f t="shared" si="0"/>
         <v>-2.1999999999999886</v>
       </c>
-      <c r="G9" s="2">
-        <v>27.44</v>
+      <c r="G9">
+        <f>ROUND((D9/1.88)/1.88,2)</f>
+        <v>27.7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -663,8 +671,9 @@
         <f t="shared" si="0"/>
         <v>-6.8000000000000114</v>
       </c>
-      <c r="G10" s="2">
-        <v>26.6</v>
+      <c r="G10">
+        <f>ROUND((D10/1.88)/1.88,2)</f>
+        <v>26.82</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -687,8 +696,9 @@
         <f t="shared" si="0"/>
         <v>1.3000000000000114</v>
       </c>
-      <c r="G11" s="2">
-        <v>26.8</v>
+      <c r="G11">
+        <f>ROUND((D11/1.88)/1.88,2)</f>
+        <v>26.99</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -711,8 +721,9 @@
         <f t="shared" si="0"/>
         <v>-2.3000000000000114</v>
       </c>
-      <c r="G12" s="2">
-        <v>26.6</v>
+      <c r="G12">
+        <f>ROUND((D12/1.88)/1.88,2)</f>
+        <v>26.68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -735,8 +746,9 @@
         <f t="shared" si="0"/>
         <v>-2.0999999999999943</v>
       </c>
-      <c r="G13" s="2">
-        <v>26.31</v>
+      <c r="G13">
+        <f>ROUND((D13/1.88)/1.88,2)</f>
+        <v>26.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating WeightMeasurement files 25/03/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FE5A61-5AE5-4725-A79A-280E5A1B12C8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A64BC1-22BD-4976-B163-37D24E674E0D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G14" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
     </row>
@@ -493,11 +493,11 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F13" si="0">E3-E2</f>
+        <f t="shared" ref="F3:F14" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
-        <f>ROUND((D3/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>29.62</v>
       </c>
     </row>
@@ -518,11 +518,11 @@
         <v>225.9</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.0999999999999943</v>
       </c>
       <c r="G4">
-        <f>ROUND((D4/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
@@ -543,11 +543,11 @@
         <v>222.8</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.0999999999999943</v>
       </c>
       <c r="G5">
-        <f>ROUND((D5/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>28.6</v>
       </c>
     </row>
@@ -568,11 +568,11 @@
         <v>220.9</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.9000000000000057</v>
       </c>
       <c r="G6">
-        <f>ROUND((D6/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>28.35</v>
       </c>
     </row>
@@ -593,11 +593,11 @@
         <v>220.9</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>ROUND((D7/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>28.35</v>
       </c>
     </row>
@@ -618,11 +618,11 @@
         <v>218</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.9000000000000057</v>
       </c>
       <c r="G8">
-        <f>ROUND((D8/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>28.01</v>
       </c>
     </row>
@@ -643,11 +643,11 @@
         <v>215.8</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.1999999999999886</v>
       </c>
       <c r="G9">
-        <f>ROUND((D9/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>27.7</v>
       </c>
     </row>
@@ -668,11 +668,11 @@
         <v>209</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.8000000000000114</v>
       </c>
       <c r="G10">
-        <f>ROUND((D10/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>26.82</v>
       </c>
     </row>
@@ -693,11 +693,11 @@
         <v>210.3</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3000000000000114</v>
       </c>
       <c r="G11">
-        <f>ROUND((D11/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>26.99</v>
       </c>
     </row>
@@ -718,11 +718,11 @@
         <v>208</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.3000000000000114</v>
       </c>
       <c r="G12">
-        <f>ROUND((D12/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>26.68</v>
       </c>
     </row>
@@ -743,12 +743,37 @@
         <v>205.9</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.0999999999999943</v>
       </c>
       <c r="G13">
-        <f>ROUND((D13/1.88)/1.88,2)</f>
+        <f t="shared" si="0"/>
         <v>26.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43184</v>
+      </c>
+      <c r="C14" s="5">
+        <v>14.11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>93.8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>207</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0999999999999943</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>26.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating WeightMeasurements file 09/04/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12FB31-65A3-4D05-BEEF-0CAE73943D01}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F715411-224A-47C4-B7B2-69C55EECB408}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
   <sheets>
     <sheet name="WeightMeasurements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G15" si="0">ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G16" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
     </row>
@@ -493,7 +493,7 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F15" si="1">E3-E2</f>
+        <f t="shared" ref="F3:F16" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
@@ -799,6 +799,31 @@
       <c r="G15">
         <f t="shared" si="0"/>
         <v>26.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43199</v>
+      </c>
+      <c r="C16" s="5">
+        <v>14.11</v>
+      </c>
+      <c r="D16" s="2">
+        <v>93.8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>207</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0999999999999943</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>26.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding BodyFat column and values to WeightMeasurements 09/04/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F715411-224A-47C4-B7B2-69C55EECB408}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BD1433-BAD9-4DE0-8B2D-7BA4523C9BAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>WeightID</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>BMI</t>
+  </si>
+  <si>
+    <t>BodyFat (%)</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,9 +433,10 @@
     <col min="5" max="5" width="13.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -451,8 +458,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -475,8 +485,11 @@
         <f t="shared" ref="G2:G16" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -500,8 +513,11 @@
         <f t="shared" si="0"/>
         <v>29.62</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -525,8 +541,11 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -550,8 +569,11 @@
         <f t="shared" si="0"/>
         <v>28.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -575,8 +597,11 @@
         <f t="shared" si="0"/>
         <v>28.35</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -600,8 +625,11 @@
         <f t="shared" si="0"/>
         <v>28.35</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -625,8 +653,11 @@
         <f t="shared" si="0"/>
         <v>28.01</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -650,8 +681,11 @@
         <f t="shared" si="0"/>
         <v>27.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -675,8 +709,11 @@
         <f t="shared" si="0"/>
         <v>26.82</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="2">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -700,8 +737,11 @@
         <f t="shared" si="0"/>
         <v>26.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="2">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -725,8 +765,11 @@
         <f t="shared" si="0"/>
         <v>26.68</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="2">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -750,8 +793,11 @@
         <f t="shared" si="0"/>
         <v>26.43</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="2">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -775,8 +821,11 @@
         <f t="shared" si="0"/>
         <v>26.54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" s="2">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -800,8 +849,11 @@
         <f t="shared" si="0"/>
         <v>26.44</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -824,6 +876,9 @@
       <c r="G16">
         <f t="shared" si="0"/>
         <v>26.54</v>
+      </c>
+      <c r="H16" s="2">
+        <v>20.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating WeightMeasurements file 22/04/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A8727-97FD-4D7B-B354-CC5855F8D8BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DC1F57-19D4-48B0-AF66-BBD0CEF3FE55}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G17" si="0">ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G18" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
       <c r="H2" t="s">
@@ -506,7 +506,7 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F17" si="1">E3-E2</f>
+        <f t="shared" ref="F3:F18" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
@@ -907,6 +907,34 @@
       </c>
       <c r="H17" s="2">
         <v>20.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43212</v>
+      </c>
+      <c r="C18" s="5">
+        <v>14.13</v>
+      </c>
+      <c r="D18" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>209</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>26.82</v>
+      </c>
+      <c r="H18" s="2">
+        <v>20.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating WeightMeasurements file 30/04/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DC1F57-19D4-48B0-AF66-BBD0CEF3FE55}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837A984-B00C-46E7-9052-CBBEBAE06C4A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G18" si="0">ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G19" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
       <c r="H2" t="s">
@@ -506,7 +506,7 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F18" si="1">E3-E2</f>
+        <f t="shared" ref="F3:F19" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
@@ -934,6 +934,34 @@
         <v>26.82</v>
       </c>
       <c r="H18" s="2">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43220</v>
+      </c>
+      <c r="C19" s="5">
+        <v>14.13</v>
+      </c>
+      <c r="D19" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>209</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>26.82</v>
+      </c>
+      <c r="H19" s="2">
         <v>20.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating WeightMeasurements file 06/05/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837A984-B00C-46E7-9052-CBBEBAE06C4A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C29932-FC74-48CD-A833-9C45CA6FE233}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G19" si="0">ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G20" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
       <c r="H2" t="s">
@@ -506,7 +506,7 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F19" si="1">E3-E2</f>
+        <f t="shared" ref="F3:F20" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
@@ -963,6 +963,34 @@
       </c>
       <c r="H19" s="2">
         <v>20.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43226</v>
+      </c>
+      <c r="C20" s="5">
+        <v>14.12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>94.3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>208</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>26.68</v>
+      </c>
+      <c r="H20" s="2">
+        <v>20.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating WeightMeasurement file 14/05/2018
</commit_message>
<xml_diff>
--- a/datasets/WeightMeasurements.xlsx
+++ b/datasets/WeightMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C29932-FC74-48CD-A833-9C45CA6FE233}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18273B88-9244-45C6-AFAE-45A86AE3168F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{9C0828BF-EE90-4966-9644-746557E4E237}"/>
   </bookViews>
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A64CFE-360B-4A31-BE7E-61C03F1787C6}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G20" si="0">ROUND((D2/1.88)/1.88,2)</f>
+        <f t="shared" ref="G2:G21" si="0">ROUND((D2/1.88)/1.88,2)</f>
         <v>29.71</v>
       </c>
       <c r="H2" t="s">
@@ -506,7 +506,7 @@
         <v>230</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F20" si="1">E3-E2</f>
+        <f t="shared" ref="F3:F21" si="1">E3-E2</f>
         <v>-1</v>
       </c>
       <c r="G3">
@@ -990,6 +990,34 @@
         <v>26.68</v>
       </c>
       <c r="H20" s="2">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43234</v>
+      </c>
+      <c r="C21" s="5">
+        <v>14.1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>93.4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>205.9</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.0999999999999943</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>26.43</v>
+      </c>
+      <c r="H21" s="2">
         <v>20.7</v>
       </c>
     </row>

</xml_diff>